<commit_message>
finish, pozostalo przetestowac postmanem
</commit_message>
<xml_diff>
--- a/asd.xlsx
+++ b/asd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zbyszard v.2\Desktop\inzynier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D37338-6B5A-4F91-A7DF-2FC8884E1DA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B1772D-F3E6-4150-9C9C-A8FDB5BFEFD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ED9A53EF-8DF2-46B6-9F6B-CC3AED4EFA87}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="18">
   <si>
     <t>ID</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>ID + ArgDate (ID+START_DT)</t>
-  </si>
-  <si>
-    <t>TODO</t>
   </si>
   <si>
     <t>endpoint</t>
@@ -527,7 +524,7 @@
   <dimension ref="C1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,7 +545,7 @@
     </row>
     <row r="2" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -693,13 +690,13 @@
     </row>
     <row r="7" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>13</v>
@@ -717,18 +714,18 @@
         <v>13</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>13</v>
@@ -746,7 +743,7 @@
         <v>13</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="3:11" x14ac:dyDescent="0.25">

</xml_diff>